<commit_message>
horizon to model area/shadow
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>11546.78839247327</v>
+        <v>11596.53993302689</v>
       </c>
     </row>
     <row r="5">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>11546.78839247327</v>
+        <v>11596.53993302689</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>8779.946007380911</v>
+        <v>8735.440285754541</v>
       </c>
     </row>
     <row r="10">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>8779.946007380911</v>
+        <v>8735.440285754541</v>
       </c>
     </row>
     <row r="11">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>8670.811607526331</v>
+        <v>8621.060066972881</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8670.811607526331</v>
+        <v>8621.060066972881</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
removed horizon added elevation calculation added area calculation based on a given time frame during shortes day / lowest sun elevation
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>11596.53993302689</v>
+        <v>13212.71166189251</v>
       </c>
     </row>
     <row r="5">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>11596.53993302689</v>
+        <v>13212.71166189251</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>8735.440285754541</v>
+        <v>7094.864641774657</v>
       </c>
     </row>
     <row r="10">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>8735.440285754541</v>
+        <v>7094.864641774657</v>
       </c>
     </row>
     <row r="11">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>8621.060066972881</v>
+        <v>7004.888338107765</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8621.060066972881</v>
+        <v>7004.888338107765</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
- correction damping - costfunctioninputs: areaUsage - design param: moduleRowSpacing
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>13212.71166189251</v>
+        <v>18732.19023536615</v>
       </c>
     </row>
     <row r="5">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>13212.71166189251</v>
+        <v>18732.19023536615</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7094.864641774657</v>
+        <v>1485.548159853576</v>
       </c>
     </row>
     <row r="10">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7094.864641774657</v>
+        <v>1485.548159853576</v>
       </c>
     </row>
     <row r="11">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7004.888338107765</v>
+        <v>1485.40976463414</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7004.888338107765</v>
+        <v>1485.40976463414</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
- add shadow model according to D1/L1 = D2/L2 --> D2 = ...
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>18732.19023536615</v>
+        <v>8602.31615895128</v>
       </c>
     </row>
     <row r="5">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>18732.19023536615</v>
+        <v>8602.31615895128</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1485.548159853576</v>
+        <v>11769.11175652173</v>
       </c>
     </row>
     <row r="10">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1485.548159853576</v>
+        <v>11769.11175652173</v>
       </c>
     </row>
     <row r="11">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1485.40976463414</v>
+        <v>11615.28384104874</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1485.40976463414</v>
+        <v>11615.28384104874</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
- update shadow model according to D1/L1 = D2/L2 --> D2 = ...
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8602.31615895128</v>
+        <v>8362.283772317136</v>
       </c>
     </row>
     <row r="5">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>8602.31615895128</v>
+        <v>8362.283772317136</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>11769.11175652173</v>
+        <v>12009.13023996808</v>
       </c>
     </row>
     <row r="10">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>11769.11175652173</v>
+        <v>12009.13023996808</v>
       </c>
     </row>
     <row r="11">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>11615.28384104874</v>
+        <v>11855.31622768284</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>11615.28384104874</v>
+        <v>11855.31622768284</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
- update shadow model - fix code
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8362.283772317136</v>
+        <v>8723.919156434198</v>
       </c>
     </row>
     <row r="5">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>8362.283772317136</v>
+        <v>8723.919156434198</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>12009.13023996808</v>
+        <v>11647.48159132677</v>
       </c>
     </row>
     <row r="10">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>12009.13023996808</v>
+        <v>11647.48159132677</v>
       </c>
     </row>
     <row r="11">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>11855.31622768284</v>
+        <v>11493.68084356613</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>11855.31622768284</v>
+        <v>11493.68084356613</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
- fix tilting - Example: NSGA multiobjective
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8723.919156434198</v>
+        <v>8831.355113164813</v>
       </c>
     </row>
     <row r="5">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>8723.919156434198</v>
+        <v>8831.355113164813</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>11647.48159132677</v>
+        <v>11540.04331251616</v>
       </c>
     </row>
     <row r="10">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>11647.48159132677</v>
+        <v>11540.04331251616</v>
       </c>
     </row>
     <row r="11">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>11493.68084356613</v>
+        <v>11386.24488683539</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>11493.68084356613</v>
+        <v>11386.24488683539</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
= ready to use for heeds
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/ConversionModel.xlsx
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8831.355113164813</v>
+        <v>13105.86444722955</v>
       </c>
     </row>
     <row r="5">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>8831.355113164813</v>
+        <v>13105.86444722955</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>11540.04331251616</v>
+        <v>7137.736985363312</v>
       </c>
     </row>
     <row r="10">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>11540.04331251616</v>
+        <v>7137.736985363312</v>
       </c>
     </row>
     <row r="11">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>11386.24488683539</v>
+        <v>7111.735552770167</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>11386.24488683539</v>
+        <v>7111.735552770167</v>
       </c>
     </row>
     <row r="16">

</xml_diff>